<commit_message>
testing the sectional loading
.
</commit_message>
<xml_diff>
--- a/dwas_mlp_output.xlsx
+++ b/dwas_mlp_output.xlsx
@@ -16,13 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>val_loss</t>
-  </si>
-  <si>
-    <t>val_mean_absolute_error</t>
-  </si>
-  <si>
-    <t>val_acc</t>
+    <t>acc</t>
   </si>
   <si>
     <t>loss</t>
@@ -31,7 +25,13 @@
     <t>mean_absolute_error</t>
   </si>
   <si>
-    <t>acc</t>
+    <t>val_acc</t>
+  </si>
+  <si>
+    <t>val_loss</t>
+  </si>
+  <si>
+    <t>val_mean_absolute_error</t>
   </si>
 </sst>
 </file>
@@ -420,22 +420,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.1402052875076021</v>
+        <v>0.6485260795641378</v>
       </c>
       <c r="C2">
-        <v>0.1402052875076021</v>
+        <v>0.2339363681013081</v>
       </c>
       <c r="D2">
-        <v>0.637566139773717</v>
+        <v>0.2339363681013081</v>
       </c>
       <c r="E2">
-        <v>0.1781897246499721</v>
+        <v>0.7328042302812848</v>
       </c>
       <c r="F2">
-        <v>0.1781897246499721</v>
+        <v>0.1964499006668727</v>
       </c>
       <c r="G2">
-        <v>0.4965986449803625</v>
+        <v>0.1964499006668727</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -443,22 +443,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.1221495544311231</v>
+        <v>0.7244897995000523</v>
       </c>
       <c r="C3">
-        <v>0.1221495544311231</v>
+        <v>0.1776597141003122</v>
       </c>
       <c r="D3">
-        <v>0.687830691772794</v>
+        <v>0.1776597141003122</v>
       </c>
       <c r="E3">
-        <v>0.1475462312736208</v>
+        <v>0.7645502632887906</v>
       </c>
       <c r="F3">
-        <v>0.1475462312736208</v>
+        <v>0.142791933049916</v>
       </c>
       <c r="G3">
-        <v>0.6065759702739802</v>
+        <v>0.142791933049916</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -466,22 +466,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.09165052608365104</v>
+        <v>0.7823129222641726</v>
       </c>
       <c r="C4">
-        <v>0.09165052608365104</v>
+        <v>0.1254619428478266</v>
       </c>
       <c r="D4">
-        <v>0.8227513195976378</v>
+        <v>0.1254619428478266</v>
       </c>
       <c r="E4">
-        <v>0.1200687657205426</v>
+        <v>0.8544973519744066</v>
       </c>
       <c r="F4">
-        <v>0.1200687657205426</v>
+        <v>0.08517111991606062</v>
       </c>
       <c r="G4">
-        <v>0.6700680312656221</v>
+        <v>0.08517111991606062</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -489,22 +489,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.05705056485360262</v>
+        <v>0.8276643965249699</v>
       </c>
       <c r="C5">
-        <v>0.05705056485360262</v>
+        <v>0.08986162239698325</v>
       </c>
       <c r="D5">
-        <v>0.835978835348099</v>
+        <v>0.08986162239698325</v>
       </c>
       <c r="E5">
-        <v>0.08420573330385074</v>
+        <v>0.8597883569500434</v>
       </c>
       <c r="F5">
-        <v>0.08420573330385074</v>
+        <v>0.05679801029581872</v>
       </c>
       <c r="G5">
-        <v>0.6927437645102305</v>
+        <v>0.05679801029581872</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -512,22 +512,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.04582747550947325</v>
+        <v>0.8605442121456</v>
       </c>
       <c r="C6">
-        <v>0.04582747550947325</v>
+        <v>0.07741538746928682</v>
       </c>
       <c r="D6">
-        <v>0.9285714210025848</v>
+        <v>0.07741538746928682</v>
       </c>
       <c r="E6">
-        <v>0.06256223664262127</v>
+        <v>0.8544973488207217</v>
       </c>
       <c r="F6">
-        <v>0.06256223664262127</v>
+        <v>0.04942771380461713</v>
       </c>
       <c r="G6">
-        <v>0.7789115619226918</v>
+        <v>0.04942771380461713</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -535,22 +535,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.04159605792827076</v>
+        <v>0.8458049856886571</v>
       </c>
       <c r="C7">
-        <v>0.04159605792827076</v>
+        <v>0.07219248730478103</v>
       </c>
       <c r="D7">
-        <v>0.941798937383783</v>
+        <v>0.07219248730478103</v>
       </c>
       <c r="E7">
-        <v>0.05538054810765108</v>
+        <v>0.8730158686007141</v>
       </c>
       <c r="F7">
-        <v>0.05538054810765108</v>
+        <v>0.04670578676950995</v>
       </c>
       <c r="G7">
-        <v>0.8265306087307919</v>
+        <v>0.04670578676950995</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -558,22 +558,22 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.03789735410027403</v>
+        <v>0.8412698395127882</v>
       </c>
       <c r="C8">
-        <v>0.03789735410027403</v>
+        <v>0.06853477337530681</v>
       </c>
       <c r="D8">
-        <v>0.90740740267688</v>
+        <v>0.06853477337530681</v>
       </c>
       <c r="E8">
-        <v>0.05094110303877297</v>
+        <v>0.8624338570725981</v>
       </c>
       <c r="F8">
-        <v>0.05094110303877297</v>
+        <v>0.04673912156392973</v>
       </c>
       <c r="G8">
-        <v>0.861677999939778</v>
+        <v>0.04673912156392973</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -581,22 +581,22 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.03688649099970621</v>
+        <v>0.8628117870581664</v>
       </c>
       <c r="C9">
-        <v>0.03688649099970621</v>
+        <v>0.06883696155821115</v>
       </c>
       <c r="D9">
-        <v>0.9391534341075433</v>
+        <v>0.06883696155821115</v>
       </c>
       <c r="E9">
-        <v>0.04845261695011267</v>
+        <v>0.8624338586494406</v>
       </c>
       <c r="F9">
-        <v>0.04845261695011267</v>
+        <v>0.04869715664437208</v>
       </c>
       <c r="G9">
-        <v>0.8696145030106006</v>
+        <v>0.04869715664437208</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -604,22 +604,22 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.03947740080692465</v>
+        <v>0.8458049833233935</v>
       </c>
       <c r="C10">
-        <v>0.03947740080692465</v>
+        <v>0.06833576908558946</v>
       </c>
       <c r="D10">
-        <v>0.9391534325307008</v>
+        <v>0.06833576908558946</v>
       </c>
       <c r="E10">
-        <v>0.04710489206117432</v>
+        <v>0.8597883553732009</v>
       </c>
       <c r="F10">
-        <v>0.04710489206117432</v>
+        <v>0.04528263484241155</v>
       </c>
       <c r="G10">
-        <v>0.8854875219922488</v>
+        <v>0.04528263484241155</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -627,22 +627,22 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.03693413500866247</v>
+        <v>0.8684807226501084</v>
       </c>
       <c r="C11">
-        <v>0.03693413500866247</v>
+        <v>0.06722350878949339</v>
       </c>
       <c r="D11">
-        <v>0.9550264490344537</v>
+        <v>0.06722350878949339</v>
       </c>
       <c r="E11">
-        <v>0.04649099244687563</v>
+        <v>0.8597883569500434</v>
       </c>
       <c r="F11">
-        <v>0.04649099244687563</v>
+        <v>0.04688214109569946</v>
       </c>
       <c r="G11">
-        <v>0.8911564575841908</v>
+        <v>0.04688214109569946</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -650,22 +650,22 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.03734829507413365</v>
+        <v>0.8594104270545804</v>
       </c>
       <c r="C12">
-        <v>0.03734829507413365</v>
+        <v>0.06408613091524766</v>
       </c>
       <c r="D12">
-        <v>0.9285714241562697</v>
+        <v>0.06408613091524766</v>
       </c>
       <c r="E12">
-        <v>0.04573449063750486</v>
+        <v>0.8624338586494406</v>
       </c>
       <c r="F12">
-        <v>0.04573449063750486</v>
+        <v>0.05066828141925196</v>
       </c>
       <c r="G12">
-        <v>0.9002267518281396</v>
+        <v>0.05066828141925196</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -673,22 +673,22 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.03753556544700312</v>
+        <v>0.8673469308011926</v>
       </c>
       <c r="C13">
-        <v>0.03753556544700312</v>
+        <v>0.0645740676476977</v>
       </c>
       <c r="D13">
-        <v>0.915343909351914</v>
+        <v>0.0645740676476977</v>
       </c>
       <c r="E13">
-        <v>0.04672209870348983</v>
+        <v>0.8597883569500434</v>
       </c>
       <c r="F13">
-        <v>0.04672209870348983</v>
+        <v>0.04672135800004951</v>
       </c>
       <c r="G13">
-        <v>0.8934240277662299</v>
+        <v>0.04672135800004951</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -696,22 +696,22 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.03588932555503946</v>
+        <v>0.8594104250272115</v>
       </c>
       <c r="C14">
-        <v>0.03588932555503946</v>
+        <v>0.06317227325336733</v>
       </c>
       <c r="D14">
-        <v>0.9365079292544612</v>
+        <v>0.06317227325336733</v>
       </c>
       <c r="E14">
-        <v>0.04432371058110612</v>
+        <v>0.8597883553732009</v>
       </c>
       <c r="F14">
-        <v>0.04432371058110612</v>
+        <v>0.04516204090779105</v>
       </c>
       <c r="G14">
-        <v>0.8866213070832683</v>
+        <v>0.04516204090779105</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -719,22 +719,22 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.03580366440669254</v>
+        <v>0.8752834426572804</v>
       </c>
       <c r="C15">
-        <v>0.03580366440669254</v>
+        <v>0.06278287619352341</v>
       </c>
       <c r="D15">
-        <v>0.9550264506112962</v>
+        <v>0.06278287619352341</v>
       </c>
       <c r="E15">
-        <v>0.04576858987951495</v>
+        <v>0.8756613718769538</v>
       </c>
       <c r="F15">
-        <v>0.04576858987951495</v>
+        <v>0.04462548879482759</v>
       </c>
       <c r="G15">
-        <v>0.9024943240375476</v>
+        <v>0.04462548879482759</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -742,22 +742,22 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.03570318221060372</v>
+        <v>0.8650793608894695</v>
       </c>
       <c r="C16">
-        <v>0.03570318221060372</v>
+        <v>0.06387534633684321</v>
       </c>
       <c r="D16">
-        <v>0.9656084621394122</v>
+        <v>0.06387534633684321</v>
       </c>
       <c r="E16">
-        <v>0.0444561225148826</v>
+        <v>0.8677248652019198</v>
       </c>
       <c r="F16">
-        <v>0.0444561225148826</v>
+        <v>0.04485266377765035</v>
       </c>
       <c r="G16">
-        <v>0.8990929653855408</v>
+        <v>0.04485266377765035</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -765,22 +765,22 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.03519799196649166</v>
+        <v>0.8571428507904347</v>
       </c>
       <c r="C17">
-        <v>0.03519799196649166</v>
+        <v>0.06122600532595127</v>
       </c>
       <c r="D17">
-        <v>0.9497354424819744</v>
+        <v>0.06122600532595127</v>
       </c>
       <c r="E17">
-        <v>0.04364877047181941</v>
+        <v>0.8650793635025227</v>
       </c>
       <c r="F17">
-        <v>0.04364877047181941</v>
+        <v>0.04338534040346978</v>
       </c>
       <c r="G17">
-        <v>0.8968253897971847</v>
+        <v>0.04338534040346978</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -788,22 +788,22 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.03558623953352845</v>
+        <v>0.8616780006155675</v>
       </c>
       <c r="C18">
-        <v>0.03558623953352845</v>
+        <v>0.06125166994475183</v>
       </c>
       <c r="D18">
-        <v>0.9417989326532555</v>
+        <v>0.06125166994475183</v>
       </c>
       <c r="E18">
-        <v>0.04289743174163122</v>
+        <v>0.8650793635025227</v>
       </c>
       <c r="F18">
-        <v>0.04289743174163122</v>
+        <v>0.04556353723324796</v>
       </c>
       <c r="G18">
-        <v>0.9081632542231727</v>
+        <v>0.04556353723324796</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -811,22 +811,22 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.03516028649986736</v>
+        <v>0.8639455735007652</v>
       </c>
       <c r="C19">
-        <v>0.03516028649986736</v>
+        <v>0.06037402545817856</v>
       </c>
       <c r="D19">
-        <v>0.9550264490344537</v>
+        <v>0.06037402545817856</v>
       </c>
       <c r="E19">
-        <v>0.04416943577175238</v>
+        <v>0.862433860226283</v>
       </c>
       <c r="F19">
-        <v>0.04416943577175238</v>
+        <v>0.04409303706356142</v>
       </c>
       <c r="G19">
-        <v>0.9024943236320738</v>
+        <v>0.04409303706356142</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -834,22 +834,22 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.03639352817344602</v>
+        <v>0.8730158670689243</v>
       </c>
       <c r="C20">
-        <v>0.03639352817344602</v>
+        <v>0.05889587356052161</v>
       </c>
       <c r="D20">
-        <v>0.9179894110513112</v>
+        <v>0.05889587356052161</v>
       </c>
       <c r="E20">
-        <v>0.04221977283354519</v>
+        <v>0.8571428552506462</v>
       </c>
       <c r="F20">
-        <v>0.04221977283354519</v>
+        <v>0.04559907312233927</v>
       </c>
       <c r="G20">
-        <v>0.8945578155604079</v>
+        <v>0.04559907312233927</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -857,22 +857,22 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.03978022464881183</v>
+        <v>0.8662131443585939</v>
       </c>
       <c r="C21">
-        <v>0.03978022464881183</v>
+        <v>0.05848183362087966</v>
       </c>
       <c r="D21">
-        <v>0.9576719523106934</v>
+        <v>0.05848183362087966</v>
       </c>
       <c r="E21">
-        <v>0.04406107021516818</v>
+        <v>0.862433860226283</v>
       </c>
       <c r="F21">
-        <v>0.04406107021516818</v>
+        <v>0.04671717172971478</v>
       </c>
       <c r="G21">
-        <v>0.9047618921922178</v>
+        <v>0.04671717172971478</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -880,22 +880,22 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.03576783270195678</v>
+        <v>0.8696145067274436</v>
       </c>
       <c r="C22">
-        <v>0.03576783270195678</v>
+        <v>0.05845955854742164</v>
       </c>
       <c r="D22">
-        <v>0.9470899392057348</v>
+        <v>0.05845955854742164</v>
       </c>
       <c r="E22">
-        <v>0.04314613651881277</v>
+        <v>0.8624338586494406</v>
       </c>
       <c r="F22">
-        <v>0.04314613651881277</v>
+        <v>0.04335810169183388</v>
       </c>
       <c r="G22">
-        <v>0.9013605375949487</v>
+        <v>0.04335810169183388</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -903,22 +903,22 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.03510457081178193</v>
+        <v>0.8786848015796029</v>
       </c>
       <c r="C23">
-        <v>0.03510457081178193</v>
+        <v>0.05910817637634115</v>
       </c>
       <c r="D23">
-        <v>0.9206349143275508</v>
+        <v>0.05910817637634115</v>
       </c>
       <c r="E23">
-        <v>0.04284186959857979</v>
+        <v>0.8571428552506462</v>
       </c>
       <c r="F23">
-        <v>0.04284186959857979</v>
+        <v>0.04385818069968274</v>
       </c>
       <c r="G23">
-        <v>0.914965978960872</v>
+        <v>0.04385818069968274</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -926,22 +926,22 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.03591007152917208</v>
+        <v>0.8662131457101732</v>
       </c>
       <c r="C24">
-        <v>0.03591007152917208</v>
+        <v>0.05932440899751759</v>
       </c>
       <c r="D24">
-        <v>0.9391534325307008</v>
+        <v>0.05932440899751759</v>
       </c>
       <c r="E24">
-        <v>0.04248515140611569</v>
+        <v>0.8650793619256801</v>
       </c>
       <c r="F24">
-        <v>0.04248515140611569</v>
+        <v>0.04331020689594052</v>
       </c>
       <c r="G24">
-        <v>0.9036281131833048</v>
+        <v>0.04331020689594052</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -949,22 +949,22 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.03684360699521171</v>
+        <v>0.8809523741944847</v>
       </c>
       <c r="C25">
-        <v>0.03684360699521171</v>
+        <v>0.05623901362558341</v>
       </c>
       <c r="D25">
-        <v>0.9444444375063377</v>
+        <v>0.05623901362558341</v>
       </c>
       <c r="E25">
-        <v>0.04265420939646611</v>
+        <v>0.862433860226283</v>
       </c>
       <c r="F25">
-        <v>0.04265420939646611</v>
+        <v>0.04400462523181602</v>
       </c>
       <c r="G25">
-        <v>0.9036281096691988</v>
+        <v>0.04400462523181602</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -972,22 +972,22 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.03521015934606708</v>
+        <v>0.8809523741944847</v>
       </c>
       <c r="C26">
-        <v>0.03521015934606708</v>
+        <v>0.0570832078182508</v>
       </c>
       <c r="D26">
-        <v>0.9365079292544612</v>
+        <v>0.0570832078182508</v>
       </c>
       <c r="E26">
-        <v>0.04143558666447934</v>
+        <v>0.8597883569500434</v>
       </c>
       <c r="F26">
-        <v>0.04143558666447934</v>
+        <v>0.0433283896436767</v>
       </c>
       <c r="G26">
-        <v>0.9115646192276018</v>
+        <v>0.0433283896436767</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -995,22 +995,22 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.0356148698480514</v>
+        <v>0.8662131484133316</v>
       </c>
       <c r="C27">
-        <v>0.0356148698480514</v>
+        <v>0.05805420705757174</v>
       </c>
       <c r="D27">
-        <v>0.9047618962469555</v>
+        <v>0.05805420705757174</v>
       </c>
       <c r="E27">
-        <v>0.0416233340772439</v>
+        <v>0.862433860226283</v>
       </c>
       <c r="F27">
-        <v>0.0416233340772439</v>
+        <v>0.0440658430258433</v>
       </c>
       <c r="G27">
-        <v>0.9081632585482262</v>
+        <v>0.0440658430258433</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1018,22 +1018,22 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.03482892224318767</v>
+        <v>0.8718820804911677</v>
       </c>
       <c r="C28">
-        <v>0.03482892224318767</v>
+        <v>0.05873115098023631</v>
       </c>
       <c r="D28">
-        <v>0.9470899407825772</v>
+        <v>0.05873115098023631</v>
       </c>
       <c r="E28">
-        <v>0.04164812452415355</v>
+        <v>0.8677248652019198</v>
       </c>
       <c r="F28">
-        <v>0.04164812452415355</v>
+        <v>0.0437937399579419</v>
       </c>
       <c r="G28">
-        <v>0.8956916020030067</v>
+        <v>0.0437937399579419</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1041,22 +1041,22 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.03572052889676006</v>
+        <v>0.8707482935079371</v>
       </c>
       <c r="C29">
-        <v>0.03572052889676006</v>
+        <v>0.05624305710297863</v>
       </c>
       <c r="D29">
-        <v>0.923280416026948</v>
+        <v>0.05624305710297863</v>
       </c>
       <c r="E29">
-        <v>0.04108626565256086</v>
+        <v>0.862433860226283</v>
       </c>
       <c r="F29">
-        <v>0.04108626565256086</v>
+        <v>0.04509334475117386</v>
       </c>
       <c r="G29">
-        <v>0.8990929640339616</v>
+        <v>0.04509334475117386</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1064,22 +1064,22 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.03544495493252441</v>
+        <v>0.8764172263967207</v>
       </c>
       <c r="C30">
-        <v>0.03544495493252441</v>
+        <v>0.05858811671062121</v>
       </c>
       <c r="D30">
-        <v>0.9444444390831801</v>
+        <v>0.05858811671062121</v>
       </c>
       <c r="E30">
-        <v>0.04233572225755845</v>
+        <v>0.862433860226283</v>
       </c>
       <c r="F30">
-        <v>0.04233572225755845</v>
+        <v>0.04311702244732746</v>
       </c>
       <c r="G30">
-        <v>0.9024943274164957</v>
+        <v>0.04311702244732746</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1087,22 +1087,22 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.03466926297301023</v>
+        <v>0.8730158680150298</v>
       </c>
       <c r="C31">
-        <v>0.03466926297301023</v>
+        <v>0.05630175254039483</v>
       </c>
       <c r="D31">
-        <v>0.9576719523106934</v>
+        <v>0.05630175254039483</v>
       </c>
       <c r="E31">
-        <v>0.04169540375454221</v>
+        <v>0.862433860226283</v>
       </c>
       <c r="F31">
-        <v>0.04169540375454221</v>
+        <v>0.04890885344021535</v>
       </c>
       <c r="G31">
-        <v>0.9058956863388182</v>
+        <v>0.04890885344021535</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1110,22 +1110,22 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.03555108391970554</v>
+        <v>0.8798185870760963</v>
       </c>
       <c r="C32">
-        <v>0.03555108391970554</v>
+        <v>0.05527254869810849</v>
       </c>
       <c r="D32">
-        <v>0.9497354440588169</v>
+        <v>0.05527254869810849</v>
       </c>
       <c r="E32">
-        <v>0.041410243459671</v>
+        <v>0.8677248652019198</v>
       </c>
       <c r="F32">
-        <v>0.041410243459671</v>
+        <v>0.04301970048004358</v>
       </c>
       <c r="G32">
-        <v>0.922902486762222</v>
+        <v>0.04301970048004358</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1133,22 +1133,22 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.03582162030593113</v>
+        <v>0.8730158686908194</v>
       </c>
       <c r="C33">
-        <v>0.03582162030593113</v>
+        <v>0.05643147025721954</v>
       </c>
       <c r="D33">
-        <v>0.9523809457582141</v>
+        <v>0.05643147025721954</v>
       </c>
       <c r="E33">
-        <v>0.04171683757973501</v>
+        <v>0.8677248652019198</v>
       </c>
       <c r="F33">
-        <v>0.04171683757973501</v>
+        <v>0.04335480003997132</v>
       </c>
       <c r="G33">
-        <v>0.9149659755819238</v>
+        <v>0.04335480003997132</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1156,22 +1156,22 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.03540207078020093</v>
+        <v>0.875283437926753</v>
       </c>
       <c r="C34">
-        <v>0.03540207078020093</v>
+        <v>0.05549544602835259</v>
       </c>
       <c r="D34">
-        <v>0.9550264490344537</v>
+        <v>0.05549544602835259</v>
       </c>
       <c r="E34">
-        <v>0.04150166464737213</v>
+        <v>0.8730158686007141</v>
       </c>
       <c r="F34">
-        <v>0.04150166464737213</v>
+        <v>0.04462635708312509</v>
       </c>
       <c r="G34">
-        <v>0.9070294698079427</v>
+        <v>0.04462635708312509</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1179,22 +1179,22 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.03472280413621948</v>
+        <v>0.8820861606370836</v>
       </c>
       <c r="C35">
-        <v>0.03472280413621948</v>
+        <v>0.05622636406025649</v>
       </c>
       <c r="D35">
-        <v>0.9444444375063377</v>
+        <v>0.05622636406025649</v>
       </c>
       <c r="E35">
-        <v>0.04110376418582977</v>
+        <v>0.8650793619256801</v>
       </c>
       <c r="F35">
-        <v>0.04110376418582977</v>
+        <v>0.04771522864226311</v>
       </c>
       <c r="G35">
-        <v>0.9183673416676165</v>
+        <v>0.04771522864226311</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1202,22 +1202,22 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.0362396881417938</v>
+        <v>0.8786848026608663</v>
       </c>
       <c r="C36">
-        <v>0.0362396881417938</v>
+        <v>0.05475998533015349</v>
       </c>
       <c r="D36">
-        <v>0.9576719538875358</v>
+        <v>0.05475998533015349</v>
       </c>
       <c r="E36">
-        <v>0.04022877117251458</v>
+        <v>0.870370366901317</v>
       </c>
       <c r="F36">
-        <v>0.04022877117251458</v>
+        <v>0.0431286519363759</v>
       </c>
       <c r="G36">
-        <v>0.9183673378831946</v>
+        <v>0.0431286519363759</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1225,22 +1225,22 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.03566416741284744</v>
+        <v>0.8775510158127938</v>
       </c>
       <c r="C37">
-        <v>0.03566416741284744</v>
+        <v>0.05525013211430335</v>
       </c>
       <c r="D37">
-        <v>0.9497354440588169</v>
+        <v>0.05525013211430335</v>
       </c>
       <c r="E37">
-        <v>0.04146749748428122</v>
+        <v>0.8571428552506462</v>
       </c>
       <c r="F37">
-        <v>0.04146749748428122</v>
+        <v>0.04425570584597096</v>
       </c>
       <c r="G37">
-        <v>0.9104308325146871</v>
+        <v>0.04425570584597096</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1248,22 +1248,22 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.03824811220839226</v>
+        <v>0.8741496548631024</v>
       </c>
       <c r="C38">
-        <v>0.03824811220839226</v>
+        <v>0.05579157561367871</v>
       </c>
       <c r="D38">
-        <v>0.9417989358069405</v>
+        <v>0.05579157561367871</v>
       </c>
       <c r="E38">
-        <v>0.04119891974897612</v>
+        <v>0.8650793619256801</v>
       </c>
       <c r="F38">
-        <v>0.04119891974897612</v>
+        <v>0.04256838499001725</v>
       </c>
       <c r="G38">
-        <v>0.9160997674308397</v>
+        <v>0.04256838499001725</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1271,22 +1271,22 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.03470720908550359</v>
+        <v>0.8832199511344201</v>
       </c>
       <c r="C39">
-        <v>0.03470720908550359</v>
+        <v>0.05553818218697226</v>
       </c>
       <c r="D39">
-        <v>0.933862427555064</v>
+        <v>0.05553818218697226</v>
       </c>
       <c r="E39">
-        <v>0.04002149891353248</v>
+        <v>0.862433860226283</v>
       </c>
       <c r="F39">
-        <v>0.04002149891353248</v>
+        <v>0.04280567773317218</v>
       </c>
       <c r="G39">
-        <v>0.9138321911666939</v>
+        <v>0.04280567773317218</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1294,22 +1294,22 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.03692282943261994</v>
+        <v>0.8798185859948329</v>
       </c>
       <c r="C40">
-        <v>0.03692282943261994</v>
+        <v>0.05361374588408708</v>
       </c>
       <c r="D40">
-        <v>0.9153439061982291</v>
+        <v>0.05361374588408708</v>
       </c>
       <c r="E40">
-        <v>0.04104491875268299</v>
+        <v>0.862433860226283</v>
       </c>
       <c r="F40">
-        <v>0.04104491875268299</v>
+        <v>0.04301337968735468</v>
       </c>
       <c r="G40">
-        <v>0.9126984047240951</v>
+        <v>0.04301337968735468</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1317,22 +1317,22 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.03458956489093089</v>
+        <v>0.8798185870760963</v>
       </c>
       <c r="C41">
-        <v>0.03458956489093089</v>
+        <v>0.05503128954714118</v>
       </c>
       <c r="D41">
-        <v>0.9523809457582141</v>
+        <v>0.05503128954714118</v>
       </c>
       <c r="E41">
-        <v>0.04116767451015054</v>
+        <v>0.8597883569500434</v>
       </c>
       <c r="F41">
-        <v>0.04116767451015054</v>
+        <v>0.04389099790542214</v>
       </c>
       <c r="G41">
-        <v>0.9058956853927128</v>
+        <v>0.04389099790542214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>